<commit_message>
Changed scale to 1to60
</commit_message>
<xml_diff>
--- a/uka15.xlsx
+++ b/uka15.xlsx
@@ -1,15 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\samfundet\Mikrolysreklamen15\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD43702-1A6C-4619-AFFB-2D1523835446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="9420"/>
+    <workbookView xWindow="45972" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="uka15" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -34,8 +53,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -517,48 +536,48 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - uthevingsfarge 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - uthevingsfarge 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - uthevingsfarge 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - uthevingsfarge 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - uthevingsfarge 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - uthevingsfarge 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - uthevingsfarge 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - uthevingsfarge 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - uthevingsfarge 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - uthevingsfarge 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - uthevingsfarge 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - uthevingsfarge 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - uthevingsfarge 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - uthevingsfarge 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - uthevingsfarge 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - uthevingsfarge 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - uthevingsfarge 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - uthevingsfarge 6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Beregning" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Dårlig" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Forklarende tekst" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="God" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Inndata" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Koblet celle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Kontrollcelle" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Merknad" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Nøytral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Overskrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Overskrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Overskrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Overskrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Tittel" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Totalt" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Utdata" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Uthevingsfarge1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Uthevingsfarge2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Uthevingsfarge3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Uthevingsfarge4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Uthevingsfarge5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Uthevingsfarge6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Varseltekst" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -828,26 +847,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:J83"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="7" width="9.140625" style="1"/>
+    <col min="2" max="7" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -880,7 +899,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -913,7 +932,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -946,7 +965,7 @@
         <v>-0.16</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -979,7 +998,7 @@
         <v>-63</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1012,7 +1031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -1039,7 +1058,7 @@
         <v>-20.2</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -1066,7 +1085,7 @@
         <v>-23.400000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -1093,7 +1112,7 @@
         <v>-22.2</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>
@@ -1120,7 +1139,7 @@
         <v>-21.2</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10</v>
       </c>
@@ -1147,7 +1166,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>11</v>
       </c>
@@ -1174,7 +1193,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12</v>
       </c>
@@ -1201,7 +1220,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>13</v>
       </c>
@@ -1228,7 +1247,7 @@
         <v>-13</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>14</v>
       </c>
@@ -1255,7 +1274,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>15</v>
       </c>
@@ -1282,7 +1301,7 @@
         <v>-17.600000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>16</v>
       </c>
@@ -1309,7 +1328,7 @@
         <v>-18.600000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>17</v>
       </c>
@@ -1336,7 +1355,7 @@
         <v>-18.600000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>18</v>
       </c>
@@ -1363,7 +1382,7 @@
         <v>-17.600000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>19</v>
       </c>
@@ -1390,7 +1409,7 @@
         <v>-15.8</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>20</v>
       </c>
@@ -1417,7 +1436,7 @@
         <v>-13</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>21</v>
       </c>
@@ -1444,7 +1463,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>22</v>
       </c>
@@ -1471,7 +1490,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>23</v>
       </c>
@@ -1498,7 +1517,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>25</v>
       </c>
@@ -1525,7 +1544,7 @@
         <v>-17.400000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>26</v>
       </c>
@@ -1552,7 +1571,7 @@
         <v>-14.200000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>27</v>
       </c>
@@ -1579,7 +1598,7 @@
         <v>-10.8</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>28</v>
       </c>
@@ -1606,7 +1625,7 @@
         <v>-7.4</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>29</v>
       </c>
@@ -1633,7 +1652,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>30</v>
       </c>
@@ -1660,7 +1679,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>31</v>
       </c>
@@ -1687,7 +1706,7 @@
         <v>-4.4000000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>32</v>
       </c>
@@ -1714,7 +1733,7 @@
         <v>-6.2</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>33</v>
       </c>
@@ -1741,7 +1760,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>34</v>
       </c>
@@ -1768,7 +1787,7 @@
         <v>-11.6</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>35</v>
       </c>
@@ -1795,7 +1814,7 @@
         <v>-14</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>36</v>
       </c>
@@ -1822,7 +1841,7 @@
         <v>-14.200000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>37</v>
       </c>
@@ -1849,7 +1868,7 @@
         <v>-10.8</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>38</v>
       </c>
@@ -1876,7 +1895,7 @@
         <v>-7.4</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>39</v>
       </c>
@@ -1903,7 +1922,7 @@
         <v>-7.6000000000000005</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>40</v>
       </c>
@@ -1930,7 +1949,7 @@
         <v>-10.6</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>41</v>
       </c>
@@ -1957,7 +1976,7 @@
         <v>-17</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>45</v>
       </c>
@@ -1984,7 +2003,7 @@
         <v>-16.8</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>46</v>
       </c>
@@ -2011,7 +2030,7 @@
         <v>-13.6</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>47</v>
       </c>
@@ -2038,7 +2057,7 @@
         <v>-10.4</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>48</v>
       </c>
@@ -2065,7 +2084,7 @@
         <v>-7.2</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>49</v>
       </c>
@@ -2092,7 +2111,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>50</v>
       </c>
@@ -2119,7 +2138,7 @@
         <v>-16.8</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>51</v>
       </c>
@@ -2146,7 +2165,7 @@
         <v>-13.6</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>52</v>
       </c>
@@ -2173,7 +2192,7 @@
         <v>-10.4</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>53</v>
       </c>
@@ -2200,7 +2219,7 @@
         <v>-7.2</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>54</v>
       </c>
@@ -2227,7 +2246,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>55</v>
       </c>
@@ -2254,7 +2273,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>56</v>
       </c>
@@ -2281,7 +2300,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>57</v>
       </c>
@@ -2308,7 +2327,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>58</v>
       </c>
@@ -2335,7 +2354,7 @@
         <v>-13.6</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>59</v>
       </c>
@@ -2362,7 +2381,7 @@
         <v>-13.6</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>65</v>
       </c>
@@ -2389,7 +2408,7 @@
         <v>-17.2</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>66</v>
       </c>
@@ -2416,7 +2435,7 @@
         <v>-14.200000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>67</v>
       </c>
@@ -2443,7 +2462,7 @@
         <v>-11.4</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>68</v>
       </c>
@@ -2470,7 +2489,7 @@
         <v>-8.4</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>69</v>
       </c>
@@ -2497,7 +2516,7 @@
         <v>-5.6000000000000005</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>70</v>
       </c>
@@ -2524,7 +2543,7 @@
         <v>-8.4</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>71</v>
       </c>
@@ -2551,7 +2570,7 @@
         <v>-11.4</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>72</v>
       </c>
@@ -2578,7 +2597,7 @@
         <v>-14.4</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>73</v>
       </c>
@@ -2605,7 +2624,7 @@
         <v>-17.400000000000002</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>74</v>
       </c>
@@ -2632,7 +2651,7 @@
         <v>-14.200000000000001</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>75</v>
       </c>
@@ -2659,7 +2678,7 @@
         <v>-11.4</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>76</v>
       </c>
@@ -2686,7 +2705,7 @@
         <v>-14.200000000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>80</v>
       </c>
@@ -2713,7 +2732,7 @@
         <v>-19.400000000000002</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>81</v>
       </c>
@@ -2740,7 +2759,7 @@
         <v>-17.2</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>82</v>
       </c>
@@ -2767,7 +2786,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>83</v>
       </c>
@@ -2794,7 +2813,7 @@
         <v>-12.8</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>84</v>
       </c>
@@ -2821,7 +2840,7 @@
         <v>-10.6</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>85</v>
       </c>
@@ -2848,7 +2867,7 @@
         <v>-8.4</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>86</v>
       </c>
@@ -2875,7 +2894,7 @@
         <v>-6.2</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>87</v>
       </c>
@@ -2902,7 +2921,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>88</v>
       </c>
@@ -2929,7 +2948,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>89</v>
       </c>
@@ -2956,7 +2975,7 @@
         <v>-6.2</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>90</v>
       </c>
@@ -2983,7 +3002,7 @@
         <v>-8.4</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>91</v>
       </c>
@@ -3010,7 +3029,7 @@
         <v>-10.6</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>92</v>
       </c>
@@ -3037,7 +3056,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>93</v>
       </c>
@@ -3064,7 +3083,7 @@
         <v>-17.2</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>94</v>
       </c>
@@ -3091,7 +3110,7 @@
         <v>-19.400000000000002</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>95</v>
       </c>

</xml_diff>